<commit_message>
another fighting fantasy item
</commit_message>
<xml_diff>
--- a/fighting-fantasy/checklist.xlsx
+++ b/fighting-fantasy/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/fighting-fantasy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39C62084-5EC7-7B4E-89AD-16F70732F86C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3C67E95-1A95-5845-9446-EBD6E43B68ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{FF4FE774-4AD2-5046-A9A2-C328E8B173B1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{FF4FE774-4AD2-5046-A9A2-C328E8B173B1}"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
   <si>
     <t>year</t>
   </si>
@@ -354,6 +354,18 @@
   </si>
   <si>
     <t>Shakaishisosha</t>
+  </si>
+  <si>
+    <t>王子の対決</t>
+  </si>
+  <si>
+    <t>Clash of Princes</t>
+  </si>
+  <si>
+    <t>clash-of-princes.jpg</t>
+  </si>
+  <si>
+    <t>slipcase set</t>
   </si>
 </sst>
 </file>
@@ -714,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E3C134-2279-5745-865F-E280D537D729}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E34"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,6 +737,7 @@
     <col min="3" max="3" width="35.83203125" customWidth="1"/>
     <col min="4" max="4" width="49.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1506,6 +1519,26 @@
         <v>105</v>
       </c>
     </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>1987</v>
+      </c>
+      <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>